<commit_message>
2nd Push with Jenkins
</commit_message>
<xml_diff>
--- a/tests/testScript/TestTemplatev2.xlsx
+++ b/tests/testScript/TestTemplatev2.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paupau/Desktop/Coding-Projects/Playwright/Laut_Paul_ProjectFolder/PlaywrightScript/tests/testScript/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9945CED-4493-1544-AF6F-CE28896CD0F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BE751B2-EDFC-B742-B2DF-B7281FFAC48B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42340" yWindow="5400" windowWidth="34220" windowHeight="15680" activeTab="6" xr2:uid="{671E243A-8591-404C-BE50-BE075CA0795F}"/>
+    <workbookView xWindow="42340" yWindow="5400" windowWidth="34220" windowHeight="15680" activeTab="3" xr2:uid="{671E243A-8591-404C-BE50-BE075CA0795F}"/>
   </bookViews>
   <sheets>
-    <sheet name="ActionList" sheetId="2" r:id="rId1"/>
-    <sheet name="Module" sheetId="4" r:id="rId2"/>
-    <sheet name="SampleTemplate" sheetId="1" r:id="rId3"/>
-    <sheet name="SauceDemoLogin_1" sheetId="5" r:id="rId4"/>
-    <sheet name="SauceDemoLogin_2" sheetId="6" r:id="rId5"/>
-    <sheet name="SauceDemoLogin_3" sheetId="7" r:id="rId6"/>
-    <sheet name="SauceDemoLogin_4" sheetId="8" r:id="rId7"/>
+    <sheet name="Objects" sheetId="12" r:id="rId1"/>
+    <sheet name="ActionList" sheetId="2" r:id="rId2"/>
+    <sheet name="Module" sheetId="4" r:id="rId3"/>
+    <sheet name="Test1" sheetId="11" r:id="rId4"/>
+    <sheet name="SauceDemoLogin_1" sheetId="5" r:id="rId5"/>
+    <sheet name="SauceDemoLogin_2" sheetId="6" r:id="rId6"/>
+    <sheet name="SauceDemoLogin_3" sheetId="7" r:id="rId7"/>
+    <sheet name="SauceDemoLogin_4" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="262">
   <si>
     <t>STEP</t>
   </si>
@@ -652,12 +653,6 @@
     <t>//*[@id="root"]/div/div[2]/div[1]</t>
   </si>
   <si>
-    <t>Validate Login Fields</t>
-  </si>
-  <si>
-    <t>Validate Username Field</t>
-  </si>
-  <si>
     <t>//*[@id="user-name"]</t>
   </si>
   <si>
@@ -709,9 +704,6 @@
     <t>UPLOADFile</t>
   </si>
   <si>
-    <t>GetModule</t>
-  </si>
-  <si>
     <t>Validate Username Field exists</t>
   </si>
   <si>
@@ -821,6 +813,21 @@
   </si>
   <si>
     <t>error_user</t>
+  </si>
+  <si>
+    <t>GETMODULE</t>
+  </si>
+  <si>
+    <t>Navigate and login to the website</t>
+  </si>
+  <si>
+    <t>Login_SauceDemo</t>
+  </si>
+  <si>
+    <t>Login_SauceDemo_Error_Start</t>
+  </si>
+  <si>
+    <t>Login_SauceDemo_Error_End</t>
   </si>
 </sst>
 </file>
@@ -853,12 +860,6 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -904,6 +905,11 @@
       <color rgb="FF000000"/>
       <name val="-webkit-standard"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri (Body)"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -944,7 +950,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -963,26 +969,27 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1297,12 +1304,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1F018FA-4988-644F-BE5B-3C98CEE142F3}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7022BDB4-A5FA-3A49-AB55-93AD33D6EB67}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:H79"/>
+  <dimension ref="A1:H78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="48.83203125" defaultRowHeight="16"/>
@@ -1311,7 +1332,7 @@
     <col min="2" max="2" width="14.1640625" style="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="43.83203125" style="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.33203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="45.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="54.5" style="13" customWidth="1"/>
     <col min="6" max="6" width="48.83203125" style="11"/>
     <col min="7" max="7" width="22" style="11" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="50.6640625" style="11" bestFit="1" customWidth="1"/>
@@ -1343,7 +1364,7 @@
         <v>6</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="G2" s="11" t="s">
         <v>8</v>
@@ -1357,7 +1378,7 @@
         <v>4</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G3" s="11" t="s">
         <v>9</v>
@@ -1368,10 +1389,10 @@
     </row>
     <row r="4" spans="1:8" ht="17">
       <c r="C4" s="11" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="G4" s="11" t="s">
         <v>10</v>
@@ -1382,10 +1403,10 @@
     </row>
     <row r="5" spans="1:8" ht="34">
       <c r="C5" s="11" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="G5" s="11" t="s">
         <v>11</v>
@@ -1396,10 +1417,10 @@
     </row>
     <row r="6" spans="1:8" ht="34">
       <c r="C6" s="11" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="G6" s="11" t="s">
         <v>12</v>
@@ -1410,10 +1431,10 @@
     </row>
     <row r="7" spans="1:8" ht="17">
       <c r="C7" s="11" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="G7" s="11" t="s">
         <v>13</v>
@@ -1424,10 +1445,10 @@
     </row>
     <row r="8" spans="1:8" ht="34">
       <c r="C8" s="11" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="G8" s="11" t="s">
         <v>14</v>
@@ -1436,44 +1457,44 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="34">
+    <row r="9" spans="1:8" ht="17">
       <c r="C9" s="11" t="s">
         <v>16</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="17">
       <c r="C10" s="11" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="17">
       <c r="C11" s="11" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="34">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="17">
       <c r="C12" s="11" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="17">
       <c r="C13" s="11" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="G13" s="11" t="s">
         <v>82</v>
@@ -1481,10 +1502,10 @@
     </row>
     <row r="14" spans="1:8" ht="18">
       <c r="C14" s="11" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G14" s="11" t="s">
         <v>15</v>
@@ -1495,10 +1516,10 @@
     </row>
     <row r="15" spans="1:8" ht="18">
       <c r="C15" s="11" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="G15" s="11" t="s">
         <v>80</v>
@@ -1506,682 +1527,682 @@
     </row>
     <row r="16" spans="1:8" ht="18">
       <c r="C16" s="11" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="17" spans="2:5" ht="18">
       <c r="C17" s="11" t="s">
-        <v>222</v>
+        <v>257</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>256</v>
+        <v>253</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="17">
+      <c r="B18" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="2:5" ht="17">
-      <c r="B19" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E19" s="12" t="s">
-        <v>5</v>
+      <c r="C19" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="2:5" ht="17">
       <c r="C20" s="11" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="2:5" ht="17">
       <c r="C21" s="11" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E21" s="13" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="2:5" ht="17">
       <c r="C22" s="11" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E22" s="13" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="2:5" ht="17">
       <c r="C23" s="11" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E23" s="13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="2:5" ht="17">
       <c r="C24" s="11" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E24" s="13" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="2:5" ht="17">
       <c r="C25" s="11" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="2:5" ht="17">
       <c r="C26" s="11" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E26" s="13" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="2:5" ht="17">
       <c r="C27" s="11" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E27" s="13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="2:5" ht="17">
       <c r="C28" s="11" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E28" s="13" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="2:5" ht="17">
       <c r="C29" s="11" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E29" s="13" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="2:5" ht="17">
       <c r="C30" s="11" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E30" s="13" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="2:5" ht="17">
       <c r="C31" s="11" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E31" s="13" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="2:5" ht="17">
       <c r="C32" s="11" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E32" s="13" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="3:5" ht="17">
       <c r="C33" s="11" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E33" s="13" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="3:5" ht="17">
       <c r="C34" s="11" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E34" s="13" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="3:5" ht="17">
       <c r="C35" s="11" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E35" s="13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="3:5" ht="17">
       <c r="C36" s="11" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E36" s="13" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="3:5" ht="17">
       <c r="C37" s="11" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E37" s="13" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="3:5" ht="17">
       <c r="C38" s="11" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E38" s="13" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="39" spans="3:5" ht="17">
       <c r="C39" s="11" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D39" s="11" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E39" s="13" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="3:5" ht="17">
       <c r="C40" s="11" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E40" s="13" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="3:5" ht="17">
       <c r="C41" s="11" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E41" s="13" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="42" spans="3:5" ht="17">
       <c r="C42" s="11" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D42" s="11" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E42" s="13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="43" spans="3:5" ht="17">
       <c r="C43" s="11" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D43" s="11" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E43" s="13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="44" spans="3:5" ht="17">
       <c r="C44" s="11" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D44" s="11" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E44" s="13" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="45" spans="3:5" ht="17">
       <c r="C45" s="11" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D45" s="11" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E45" s="13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="46" spans="3:5" ht="17">
       <c r="C46" s="11" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="E46" s="13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="47" spans="3:5" ht="17">
       <c r="C47" s="11" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E47" s="13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="48" spans="3:5" ht="17">
       <c r="C48" s="11" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D48" s="11" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E48" s="13" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="49" spans="3:5" ht="17">
       <c r="C49" s="11" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D49" s="11" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E49" s="13" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="50" spans="3:5" ht="17">
       <c r="C50" s="11" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D50" s="11" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E50" s="13" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="51" spans="3:5" ht="17">
       <c r="C51" s="11" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D51" s="11" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E51" s="13" t="s">
-        <v>48</v>
+        <v>246</v>
       </c>
     </row>
     <row r="52" spans="3:5" ht="17">
       <c r="C52" s="11" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D52" s="11" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E52" s="13" t="s">
-        <v>249</v>
+        <v>75</v>
       </c>
     </row>
     <row r="53" spans="3:5" ht="17">
       <c r="C53" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D53" s="11" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E53" s="13" t="s">
-        <v>75</v>
+        <v>49</v>
       </c>
     </row>
     <row r="54" spans="3:5" ht="17">
       <c r="C54" s="11" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D54" s="11" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E54" s="13" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="55" spans="3:5" ht="17">
       <c r="C55" s="11" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D55" s="11" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E55" s="13" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="56" spans="3:5" ht="17">
       <c r="C56" s="11" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D56" s="11" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E56" s="13" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="57" spans="3:5" ht="17">
       <c r="C57" s="11" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D57" s="11" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E57" s="13" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="58" spans="3:5" ht="17">
       <c r="C58" s="11" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D58" s="11" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E58" s="13" t="s">
-        <v>53</v>
+        <v>247</v>
       </c>
     </row>
     <row r="59" spans="3:5" ht="17">
       <c r="C59" s="11" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D59" s="11" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E59" s="13" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="60" spans="3:5" ht="17">
       <c r="C60" s="11" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D60" s="11" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E60" s="13" t="s">
-        <v>251</v>
+        <v>76</v>
       </c>
     </row>
     <row r="61" spans="3:5" ht="17">
       <c r="C61" s="11" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D61" s="11" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E61" s="13" t="s">
-        <v>76</v>
+        <v>249</v>
       </c>
     </row>
     <row r="62" spans="3:5" ht="17">
       <c r="C62" s="11" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D62" s="11" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E62" s="13" t="s">
-        <v>252</v>
+        <v>54</v>
       </c>
     </row>
     <row r="63" spans="3:5" ht="17">
       <c r="C63" s="11" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D63" s="11" t="s">
         <v>125</v>
       </c>
       <c r="E63" s="13" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="64" spans="3:5" ht="17">
       <c r="C64" s="11" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D64" s="11" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E64" s="13" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="65" spans="3:5" ht="17">
       <c r="C65" s="11" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D65" s="11" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E65" s="13" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="66" spans="3:5" ht="34">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="66" spans="3:5" ht="17">
       <c r="C66" s="11" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D66" s="11" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E66" s="13" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="67" spans="3:5" ht="17">
       <c r="C67" s="11" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D67" s="11" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E67" s="13" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="68" spans="3:5" ht="17">
       <c r="C68" s="11" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D68" s="11" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E68" s="13" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="69" spans="3:5" ht="17">
       <c r="C69" s="11" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D69" s="11" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E69" s="13" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="70" spans="3:5" ht="17">
       <c r="C70" s="11" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D70" s="11" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E70" s="13" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="71" spans="3:5" ht="17">
       <c r="C71" s="11" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D71" s="11" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E71" s="13" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="72" spans="3:5" ht="17">
       <c r="C72" s="11" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D72" s="11" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E72" s="13" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="73" spans="3:5" ht="17">
       <c r="C73" s="11" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D73" s="11" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E73" s="13" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="74" spans="3:5" ht="17">
       <c r="C74" s="11" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D74" s="11" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E74" s="13" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="75" spans="3:5" ht="17">
       <c r="C75" s="11" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D75" s="11" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E75" s="13" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
     </row>
     <row r="76" spans="3:5" ht="17">
       <c r="C76" s="11" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D76" s="11" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E76" s="13" t="s">
-        <v>48</v>
+        <v>67</v>
       </c>
     </row>
     <row r="77" spans="3:5" ht="17">
       <c r="C77" s="11" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D77" s="11" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E77" s="13" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
     </row>
     <row r="78" spans="3:5" ht="17">
-      <c r="C78" s="11" t="s">
-        <v>199</v>
-      </c>
       <c r="D78" s="11" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E78" s="13" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="79" spans="3:5" ht="17">
-      <c r="D79" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="E79" s="13" t="s">
         <v>60</v>
       </c>
     </row>
@@ -2191,13 +2212,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ABC7BA5-84D7-D442-947E-A7EF9E248EC3}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2213,7 +2234,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="7" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -2236,7 +2257,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2261,7 +2282,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>203</v>
+        <v>221</v>
       </c>
       <c r="D4" t="s">
         <v>150</v>
@@ -2278,7 +2299,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>204</v>
+        <v>220</v>
       </c>
       <c r="D5" t="s">
         <v>150</v>
@@ -2287,7 +2308,7 @@
         <v>15</v>
       </c>
       <c r="F5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -2295,7 +2316,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D6" t="s">
         <v>145</v>
@@ -2304,30 +2325,359 @@
         <v>15</v>
       </c>
       <c r="F6" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" t="s">
-        <v>209</v>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>222</v>
+      </c>
+      <c r="D7" t="s">
+        <v>150</v>
+      </c>
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>224</v>
+      </c>
+      <c r="D8" t="s">
+        <v>145</v>
+      </c>
+      <c r="E8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="18">
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>225</v>
+      </c>
+      <c r="D9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" t="s">
+        <v>203</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="18">
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>227</v>
+      </c>
+      <c r="D10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" t="s">
+        <v>223</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="B11">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>229</v>
+      </c>
+      <c r="D11" t="s">
+        <v>150</v>
+      </c>
+      <c r="E11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
+        <v>231</v>
+      </c>
+      <c r="D12" t="s">
+        <v>208</v>
+      </c>
+      <c r="E12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="B13">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>233</v>
+      </c>
+      <c r="D13" t="s">
+        <v>150</v>
+      </c>
+      <c r="E13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>81</v>
+      </c>
+      <c r="D16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" t="s">
+        <v>80</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>221</v>
+      </c>
+      <c r="D17" t="s">
+        <v>150</v>
+      </c>
+      <c r="E17" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18" t="s">
+        <v>220</v>
+      </c>
+      <c r="D18" t="s">
+        <v>150</v>
+      </c>
+      <c r="E18" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="B19">
+        <v>4</v>
+      </c>
+      <c r="C19" t="s">
+        <v>204</v>
+      </c>
+      <c r="D19" t="s">
+        <v>145</v>
+      </c>
+      <c r="E19" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="B20">
+        <v>5</v>
+      </c>
+      <c r="C20" t="s">
+        <v>222</v>
+      </c>
+      <c r="D20" t="s">
+        <v>150</v>
+      </c>
+      <c r="E20" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="B21">
+        <v>6</v>
+      </c>
+      <c r="C21" t="s">
+        <v>224</v>
+      </c>
+      <c r="D21" t="s">
+        <v>145</v>
+      </c>
+      <c r="E21" t="s">
+        <v>15</v>
+      </c>
+      <c r="F21" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="18">
+      <c r="B22">
+        <v>7</v>
+      </c>
+      <c r="C22" t="s">
+        <v>225</v>
+      </c>
+      <c r="D22" t="s">
+        <v>4</v>
+      </c>
+      <c r="E22" t="s">
+        <v>15</v>
+      </c>
+      <c r="F22" t="s">
+        <v>203</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="18">
+      <c r="B23">
+        <v>8</v>
+      </c>
+      <c r="C23" t="s">
+        <v>227</v>
+      </c>
+      <c r="D23" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" t="s">
+        <v>15</v>
+      </c>
+      <c r="F23" t="s">
+        <v>223</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="B24">
+        <v>9</v>
+      </c>
+      <c r="C24" t="s">
+        <v>229</v>
+      </c>
+      <c r="D24" t="s">
+        <v>150</v>
+      </c>
+      <c r="E24" t="s">
+        <v>15</v>
+      </c>
+      <c r="F24" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="B25">
+        <v>10</v>
+      </c>
+      <c r="C25" t="s">
+        <v>231</v>
+      </c>
+      <c r="D25" t="s">
+        <v>208</v>
+      </c>
+      <c r="E25" t="s">
+        <v>15</v>
+      </c>
+      <c r="F25" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="B26">
+        <v>11</v>
+      </c>
+      <c r="C26" t="s">
+        <v>233</v>
+      </c>
+      <c r="D26" t="s">
+        <v>150</v>
+      </c>
+      <c r="E26" t="s">
+        <v>15</v>
+      </c>
+      <c r="F26" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" t="s">
+        <v>261</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CF1766CD-07AE-3845-A6B0-1B0947CEDF6D}">
           <x14:formula1>
-            <xm:f>ActionList!$G$2:$G$34</xm:f>
+            <xm:f>ActionList!$G$2:$G$33</xm:f>
           </x14:formula1>
-          <xm:sqref>E3:E6</xm:sqref>
+          <xm:sqref>E3:E13 E16:E26</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{79728A79-A596-3D4A-A316-83B51DE59B81}">
           <x14:formula1>
-            <xm:f>ActionList!$C$2:$C$78</xm:f>
+            <xm:f>ActionList!$C$2:$C$77</xm:f>
           </x14:formula1>
-          <xm:sqref>D3:D6</xm:sqref>
+          <xm:sqref>D3:D13 D16:D26</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2335,15 +2685,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5680E214-49C5-A34D-8D54-6D8EA56B99C7}">
-  <sheetPr codeName="Sheet3">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0EDB696-AB8A-D54C-B2ED-056F58593EDC}">
+  <sheetPr>
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
   <dimension ref="A1:H1048562"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="16" zeroHeight="1"/>
@@ -2383,195 +2733,31 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>81</v>
+        <v>258</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>80</v>
-      </c>
+        <v>257</v>
+      </c>
+      <c r="D2"/>
       <c r="E2"/>
-      <c r="F2" s="6" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>224</v>
-      </c>
-      <c r="C3" t="s">
-        <v>150</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>223</v>
-      </c>
-      <c r="C4" t="s">
-        <v>150</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>206</v>
-      </c>
-      <c r="C5" t="s">
-        <v>145</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>225</v>
-      </c>
-      <c r="C6" t="s">
-        <v>150</v>
-      </c>
-      <c r="D6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>227</v>
-      </c>
-      <c r="C7" t="s">
-        <v>145</v>
-      </c>
-      <c r="D7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" t="s">
-        <v>226</v>
-      </c>
+      <c r="F2" s="16" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6"/>
+    <row r="4" spans="1:6"/>
+    <row r="5" spans="1:6"/>
+    <row r="6" spans="1:6"/>
+    <row r="7" spans="1:6" ht="18">
+      <c r="F7" s="8"/>
     </row>
     <row r="8" spans="1:6" ht="18">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>228</v>
-      </c>
-      <c r="C8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" t="s">
-        <v>205</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="18">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>230</v>
-      </c>
-      <c r="C9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" t="s">
-        <v>226</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>232</v>
-      </c>
-      <c r="C10" t="s">
-        <v>150</v>
-      </c>
-      <c r="D10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>234</v>
-      </c>
-      <c r="C11" t="s">
-        <v>210</v>
-      </c>
-      <c r="D11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>236</v>
-      </c>
-      <c r="C12" t="s">
-        <v>150</v>
-      </c>
-      <c r="D12" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" t="s">
-        <v>235</v>
-      </c>
-    </row>
+      <c r="F8" s="8"/>
+    </row>
+    <row r="9" spans="1:6"/>
+    <row r="10" spans="1:6"/>
+    <row r="11" spans="1:6"/>
+    <row r="12" spans="1:6"/>
     <row r="13" spans="1:6"/>
     <row r="14" spans="1:6"/>
     <row r="15" spans="1:6"/>
@@ -2583,7 +2769,7 @@
     <row r="21"/>
     <row r="22"/>
     <row r="23"/>
-    <row r="24"/>
+    <row r="25"/>
     <row r="26"/>
     <row r="27"/>
     <row r="28"/>
@@ -2591,38 +2777,38 @@
     <row r="30"/>
     <row r="31"/>
     <row r="32"/>
-    <row r="42"/>
-    <row r="1048538"/>
+    <row r="41"/>
+    <row r="1048537"/>
+    <row r="1048553"/>
     <row r="1048554"/>
-    <row r="1048555"/>
+    <row r="1048558"/>
     <row r="1048559"/>
     <row r="1048560"/>
     <row r="1048561"/>
     <row r="1048562"/>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5D493A76-68D0-254E-89B8-D6555B575E6C}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B032A48B-8DD8-0E49-9C50-BB1B03800054}">
           <x14:formula1>
-            <xm:f>ActionList!$D$2:$D$90</xm:f>
+            <xm:f>ActionList!$D$2:$D$89</xm:f>
           </x14:formula1>
-          <xm:sqref>C13:C1048576</xm:sqref>
+          <xm:sqref>C12:C1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{008490DA-7504-5646-9AD4-E89B7689A260}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EDC5A06D-4AA9-D040-A9D3-52CE7CA94438}">
           <x14:formula1>
-            <xm:f>ActionList!$G$2:$G$34</xm:f>
+            <xm:f>ActionList!$G$2:$G$33</xm:f>
           </x14:formula1>
           <xm:sqref>D2:D1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{086BF5C2-A369-564D-8984-D71A62D6729E}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4C9004C3-B3DA-204A-ABD1-0A125C8E796F}">
           <x14:formula1>
-            <xm:f>ActionList!$C$2:$C$78</xm:f>
+            <xm:f>ActionList!$C$2:$C$77</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C12</xm:sqref>
+          <xm:sqref>C2:C11</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2630,7 +2816,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BFFF14E-0430-3540-A122-C8A434C4D519}">
   <sheetPr codeName="Sheet4">
     <tabColor rgb="FF7030A0"/>
@@ -2638,7 +2824,7 @@
   <dimension ref="A1:H1048562"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="16" zeroHeight="1"/>
@@ -2696,7 +2882,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C3" t="s">
         <v>150</v>
@@ -2713,7 +2899,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C4" t="s">
         <v>150</v>
@@ -2722,7 +2908,7 @@
         <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2730,7 +2916,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C5" t="s">
         <v>145</v>
@@ -2739,7 +2925,7 @@
         <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -2747,7 +2933,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C6" t="s">
         <v>150</v>
@@ -2756,7 +2942,7 @@
         <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2764,7 +2950,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C7" t="s">
         <v>145</v>
@@ -2773,7 +2959,7 @@
         <v>15</v>
       </c>
       <c r="E7" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="18">
@@ -2781,7 +2967,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -2790,10 +2976,10 @@
         <v>15</v>
       </c>
       <c r="E8" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="18">
@@ -2801,7 +2987,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -2810,10 +2996,10 @@
         <v>15</v>
       </c>
       <c r="E9" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -2821,7 +3007,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C10" t="s">
         <v>150</v>
@@ -2830,7 +3016,7 @@
         <v>15</v>
       </c>
       <c r="E10" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -2838,16 +3024,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C11" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D11" t="s">
         <v>15</v>
       </c>
       <c r="E11" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -2855,7 +3041,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C12" t="s">
         <v>150</v>
@@ -2864,7 +3050,7 @@
         <v>15</v>
       </c>
       <c r="E12" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="13" spans="1:6"/>
@@ -2902,19 +3088,19 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{12AA1206-B45D-AD4E-A346-4BA578028D10}">
           <x14:formula1>
-            <xm:f>ActionList!$C$2:$C$78</xm:f>
+            <xm:f>ActionList!$C$2:$C$77</xm:f>
           </x14:formula1>
           <xm:sqref>C2:C12</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{176B958C-E235-9242-B28E-ABB4F5CDE65B}">
           <x14:formula1>
-            <xm:f>ActionList!$G$2:$G$34</xm:f>
+            <xm:f>ActionList!$G$2:$G$33</xm:f>
           </x14:formula1>
           <xm:sqref>D2:D1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{630B7E57-3322-C74A-8D37-06D3C51EAFE3}">
           <x14:formula1>
-            <xm:f>ActionList!$D$2:$D$90</xm:f>
+            <xm:f>ActionList!$D$2:$D$89</xm:f>
           </x14:formula1>
           <xm:sqref>C13:C1048576</xm:sqref>
         </x14:dataValidation>
@@ -2924,7 +3110,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B18B8F0-9982-1A49-83DC-1B28B000D5EE}">
   <sheetPr codeName="Sheet5">
     <tabColor rgb="FF7030A0"/>
@@ -2932,7 +3118,7 @@
   <dimension ref="A1:H1048562"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="A2" sqref="A2:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="16" zeroHeight="1"/>
@@ -2990,7 +3176,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C3" t="s">
         <v>150</v>
@@ -3007,7 +3193,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C4" t="s">
         <v>150</v>
@@ -3016,7 +3202,7 @@
         <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -3024,7 +3210,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C5" t="s">
         <v>145</v>
@@ -3033,7 +3219,7 @@
         <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -3041,7 +3227,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C6" t="s">
         <v>150</v>
@@ -3050,7 +3236,7 @@
         <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -3058,7 +3244,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C7" t="s">
         <v>145</v>
@@ -3067,7 +3253,7 @@
         <v>15</v>
       </c>
       <c r="E7" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="18">
@@ -3075,7 +3261,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -3084,10 +3270,10 @@
         <v>15</v>
       </c>
       <c r="E8" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="18">
@@ -3095,7 +3281,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -3104,10 +3290,10 @@
         <v>15</v>
       </c>
       <c r="E9" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -3115,7 +3301,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C10" t="s">
         <v>150</v>
@@ -3124,7 +3310,7 @@
         <v>15</v>
       </c>
       <c r="E10" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -3132,16 +3318,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C11" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D11" t="s">
         <v>15</v>
       </c>
       <c r="E11" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -3149,7 +3335,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C12" t="s">
         <v>150</v>
@@ -3158,7 +3344,7 @@
         <v>15</v>
       </c>
       <c r="E12" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="13" spans="1:6"/>
@@ -3196,19 +3382,19 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FC9B30DA-0BE6-EB49-8315-EE7FE942AAA2}">
           <x14:formula1>
-            <xm:f>ActionList!$D$2:$D$90</xm:f>
+            <xm:f>ActionList!$D$2:$D$89</xm:f>
           </x14:formula1>
           <xm:sqref>C13:C1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5CC9CB10-6F83-BA4D-9348-8D7B45667D73}">
           <x14:formula1>
-            <xm:f>ActionList!$G$2:$G$34</xm:f>
+            <xm:f>ActionList!$G$2:$G$33</xm:f>
           </x14:formula1>
           <xm:sqref>D2:D1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4E16D7B0-A620-7C4E-A7D5-217892F182A9}">
           <x14:formula1>
-            <xm:f>ActionList!$C$2:$C$78</xm:f>
+            <xm:f>ActionList!$C$2:$C$77</xm:f>
           </x14:formula1>
           <xm:sqref>C2:C12</xm:sqref>
         </x14:dataValidation>
@@ -3218,7 +3404,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3980E944-7AA5-0C41-A89B-455BF2CFBA2E}">
   <sheetPr codeName="Sheet6">
     <tabColor rgb="FF7030A0"/>
@@ -3284,7 +3470,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C3" t="s">
         <v>150</v>
@@ -3301,7 +3487,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C4" t="s">
         <v>150</v>
@@ -3310,7 +3496,7 @@
         <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -3318,7 +3504,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C5" t="s">
         <v>145</v>
@@ -3327,7 +3513,7 @@
         <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -3335,7 +3521,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C6" t="s">
         <v>150</v>
@@ -3344,7 +3530,7 @@
         <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -3352,7 +3538,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C7" t="s">
         <v>145</v>
@@ -3361,7 +3547,7 @@
         <v>15</v>
       </c>
       <c r="E7" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="18">
@@ -3369,7 +3555,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -3378,10 +3564,10 @@
         <v>15</v>
       </c>
       <c r="E8" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="18">
@@ -3389,7 +3575,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -3398,10 +3584,10 @@
         <v>15</v>
       </c>
       <c r="E9" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -3409,7 +3595,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C10" t="s">
         <v>150</v>
@@ -3418,7 +3604,7 @@
         <v>15</v>
       </c>
       <c r="E10" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -3426,16 +3612,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C11" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D11" t="s">
         <v>15</v>
       </c>
       <c r="E11" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -3443,7 +3629,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C12" t="s">
         <v>150</v>
@@ -3452,7 +3638,7 @@
         <v>15</v>
       </c>
       <c r="E12" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="13" spans="1:6"/>
@@ -3490,19 +3676,19 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{23972891-D4D3-664D-8D33-8225BC093B04}">
           <x14:formula1>
-            <xm:f>ActionList!$C$2:$C$78</xm:f>
+            <xm:f>ActionList!$C$2:$C$77</xm:f>
           </x14:formula1>
           <xm:sqref>C2:C12</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D0449DAC-1450-5746-AA9E-FDE8D1F23495}">
           <x14:formula1>
-            <xm:f>ActionList!$G$2:$G$34</xm:f>
+            <xm:f>ActionList!$G$2:$G$33</xm:f>
           </x14:formula1>
           <xm:sqref>D2:D1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{129791D0-A6EA-0343-8BED-5161B956623E}">
           <x14:formula1>
-            <xm:f>ActionList!$D$2:$D$90</xm:f>
+            <xm:f>ActionList!$D$2:$D$89</xm:f>
           </x14:formula1>
           <xm:sqref>C13:C1048576</xm:sqref>
         </x14:dataValidation>
@@ -3512,15 +3698,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2DE3458-E05A-3B40-8B6C-CB67612CC281}">
   <sheetPr>
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
   <dimension ref="A1:H1048562"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="16" zeroHeight="1"/>
@@ -3578,7 +3764,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C3" t="s">
         <v>150</v>
@@ -3595,7 +3781,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C4" t="s">
         <v>150</v>
@@ -3604,7 +3790,7 @@
         <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -3612,7 +3798,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C5" t="s">
         <v>145</v>
@@ -3621,7 +3807,7 @@
         <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -3629,7 +3815,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C6" t="s">
         <v>150</v>
@@ -3638,7 +3824,7 @@
         <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -3646,7 +3832,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C7" t="s">
         <v>145</v>
@@ -3655,7 +3841,7 @@
         <v>15</v>
       </c>
       <c r="E7" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="18">
@@ -3663,7 +3849,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -3672,10 +3858,10 @@
         <v>15</v>
       </c>
       <c r="E8" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="18">
@@ -3683,7 +3869,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -3692,10 +3878,10 @@
         <v>15</v>
       </c>
       <c r="E9" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -3703,7 +3889,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C10" t="s">
         <v>150</v>
@@ -3712,7 +3898,7 @@
         <v>15</v>
       </c>
       <c r="E10" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -3720,16 +3906,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C11" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D11" t="s">
         <v>15</v>
       </c>
       <c r="E11" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -3737,7 +3923,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C12" t="s">
         <v>150</v>
@@ -3746,7 +3932,7 @@
         <v>15</v>
       </c>
       <c r="E12" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="13" spans="1:6"/>
@@ -3784,19 +3970,19 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{49CE370A-D2ED-8842-93FA-DBD1D726CB2C}">
           <x14:formula1>
-            <xm:f>ActionList!$D$2:$D$90</xm:f>
+            <xm:f>ActionList!$D$2:$D$89</xm:f>
           </x14:formula1>
           <xm:sqref>C13:C1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{58DFFC6C-EB7E-A04A-A3EF-E33B4DC28961}">
           <x14:formula1>
-            <xm:f>ActionList!$G$2:$G$34</xm:f>
+            <xm:f>ActionList!$G$2:$G$33</xm:f>
           </x14:formula1>
           <xm:sqref>D2:D1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{76770B72-5C1D-A846-96D3-DA9EC5C09A56}">
           <x14:formula1>
-            <xm:f>ActionList!$C$2:$C$78</xm:f>
+            <xm:f>ActionList!$C$2:$C$77</xm:f>
           </x14:formula1>
           <xm:sqref>C2:C12</xm:sqref>
         </x14:dataValidation>

</xml_diff>